<commit_message>
Update Lady Bayning Sheets spreadsheet
</commit_message>
<xml_diff>
--- a/Locations/Lady-Bayning-Sheets.xlsx
+++ b/Locations/Lady-Bayning-Sheets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\BritishRainfall\Locations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F52E75-D719-4EA2-995B-AFC08C98F37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C115EB3-4FC8-45B1-8D82-257D38AD41DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C570D48-7BD6-4CE8-84C3-681D1BDED94F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="101">
   <si>
     <t>Volume</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Suffolk</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>BROME NEAR EYE SUFFOLK</t>
   </si>
   <si>
@@ -335,6 +332,12 @@
   </si>
   <si>
     <t>1855/12</t>
+  </si>
+  <si>
+    <t>EYE-BROME</t>
+  </si>
+  <si>
+    <t>V2/DATA</t>
   </si>
 </sst>
 </file>
@@ -688,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC946CF-DF31-4BB3-BD47-4C722A3F2BEC}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,13 +1187,13 @@
         <v>28</v>
       </c>
       <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" t="s">
         <v>62</v>
-      </c>
-      <c r="I9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" t="s">
-        <v>63</v>
       </c>
       <c r="K9">
         <v>10</v>
@@ -1199,7 +1202,7 @@
         <v>1840</v>
       </c>
       <c r="M9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N9">
         <v>38</v>
@@ -1211,11 +1214,11 @@
         <v>31.7</v>
       </c>
       <c r="Q9" t="s">
+        <v>64</v>
+      </c>
+      <c r="R9" t="s">
         <v>65</v>
       </c>
-      <c r="R9" t="s">
-        <v>66</v>
-      </c>
       <c r="S9">
         <v>0</v>
       </c>
@@ -1223,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="W9" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -1252,10 +1255,10 @@
         <v>29</v>
       </c>
       <c r="I10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" t="s">
         <v>67</v>
-      </c>
-      <c r="J10" t="s">
-        <v>68</v>
       </c>
       <c r="K10">
         <v>10</v>
@@ -1264,7 +1267,7 @@
         <v>1840</v>
       </c>
       <c r="M10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N10">
         <v>46</v>
@@ -1276,10 +1279,10 @@
         <v>38.299999999999997</v>
       </c>
       <c r="Q10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10" t="s">
         <v>70</v>
-      </c>
-      <c r="R10" t="s">
-        <v>71</v>
       </c>
       <c r="S10">
         <v>2</v>
@@ -1296,7 +1299,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11">
         <v>181</v>
@@ -1305,7 +1308,7 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
         <v>26</v>
@@ -1320,10 +1323,10 @@
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K11">
         <v>10</v>
@@ -1332,7 +1335,7 @@
         <v>1850</v>
       </c>
       <c r="M11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N11">
         <v>117</v>
@@ -1344,10 +1347,10 @@
         <v>97.5</v>
       </c>
       <c r="Q11" t="s">
+        <v>75</v>
+      </c>
+      <c r="R11" t="s">
         <v>76</v>
-      </c>
-      <c r="R11" t="s">
-        <v>77</v>
       </c>
       <c r="S11">
         <v>9</v>
@@ -1364,7 +1367,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12">
         <v>118</v>
@@ -1373,7 +1376,7 @@
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
@@ -1388,10 +1391,10 @@
         <v>29</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K12">
         <v>10</v>
@@ -1400,7 +1403,7 @@
         <v>1860</v>
       </c>
       <c r="M12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N12">
         <v>120</v>
@@ -1412,10 +1415,10 @@
         <v>100</v>
       </c>
       <c r="Q12" t="s">
+        <v>80</v>
+      </c>
+      <c r="R12" t="s">
         <v>81</v>
-      </c>
-      <c r="R12" t="s">
-        <v>82</v>
       </c>
       <c r="S12">
         <v>10</v>
@@ -1432,7 +1435,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13">
         <v>29</v>
@@ -1441,7 +1444,7 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
         <v>26</v>
@@ -1456,10 +1459,10 @@
         <v>29</v>
       </c>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K13">
         <v>10</v>
@@ -1468,7 +1471,7 @@
         <v>1870</v>
       </c>
       <c r="M13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N13">
         <v>120</v>
@@ -1480,10 +1483,10 @@
         <v>100</v>
       </c>
       <c r="Q13" t="s">
+        <v>85</v>
+      </c>
+      <c r="R13" t="s">
         <v>86</v>
-      </c>
-      <c r="R13" t="s">
-        <v>87</v>
       </c>
       <c r="S13">
         <v>10</v>
@@ -1500,7 +1503,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14">
         <v>34</v>
@@ -1509,7 +1512,7 @@
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
         <v>26</v>
@@ -1524,10 +1527,10 @@
         <v>29</v>
       </c>
       <c r="I14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K14">
         <v>10</v>
@@ -1536,7 +1539,7 @@
         <v>1880</v>
       </c>
       <c r="M14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N14">
         <v>95</v>
@@ -1548,10 +1551,10 @@
         <v>79.2</v>
       </c>
       <c r="Q14" t="s">
+        <v>90</v>
+      </c>
+      <c r="R14" t="s">
         <v>91</v>
-      </c>
-      <c r="R14" t="s">
-        <v>92</v>
       </c>
       <c r="S14">
         <v>7</v>
@@ -1592,10 +1595,10 @@
         <v>29</v>
       </c>
       <c r="I16" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" t="s">
         <v>93</v>
-      </c>
-      <c r="J16" t="s">
-        <v>94</v>
       </c>
       <c r="K16">
         <v>10</v>
@@ -1604,7 +1607,7 @@
         <v>1840</v>
       </c>
       <c r="M16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N16">
         <v>24</v>
@@ -1616,10 +1619,10 @@
         <v>20</v>
       </c>
       <c r="Q16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S16">
         <v>6</v>
@@ -1636,7 +1639,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17">
         <v>182</v>
@@ -1645,7 +1648,7 @@
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
         <v>26</v>
@@ -1660,10 +1663,10 @@
         <v>29</v>
       </c>
       <c r="I17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K17">
         <v>10</v>
@@ -1672,7 +1675,7 @@
         <v>1850</v>
       </c>
       <c r="M17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N17">
         <v>72</v>
@@ -1684,10 +1687,10 @@
         <v>60</v>
       </c>
       <c r="Q17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S17">
         <v>4</v>

</xml_diff>